<commit_message>
SEC-587 Made the height equal the width in the launch file, added colors to the xlsx
</commit_message>
<xml_diff>
--- a/ros_pkg/securbot_pkg/launch/includes/OccupancyGridValidator.xlsx
+++ b/ros_pkg/securbot_pkg/launch/includes/OccupancyGridValidator.xlsx
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t xml:space="preserve">RTAB-MAP</t>
   </si>
@@ -142,6 +142,34 @@
   </si>
   <si>
     <t xml:space="preserve">Launch</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ne modifier que les cases en bleu, les grises sont calculées </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">automatiques</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Les cases en jaune peuvent être modifiées, mais prendre les valeurs dans rviz, ces valeurs ne peuvent pas être modifier par nous...</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Var</t>
@@ -178,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -200,13 +228,43 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF685"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7DA7D8"/>
+        <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -243,9 +301,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -257,6 +331,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF7DA7D8"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFF685"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -268,7 +402,7 @@
   <dimension ref="C4:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,19 +433,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>421</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>421</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>0.05</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>-10.525</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>-10.525</v>
       </c>
     </row>
@@ -338,96 +472,123 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="2" t="n">
         <v>25</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="3" t="n">
         <f aca="false">E14*C14/2</f>
         <v>500</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="3" t="n">
         <f aca="false">E14*C14/2</f>
         <v>500</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="n">
         <f aca="false">G7*E14+G14</f>
         <v>236.875</v>
       </c>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D22" s="3" t="n">
         <f aca="false">F7*E14+F14</f>
         <v>236.875</v>
       </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D23" s="3" t="n">
         <f aca="false">G14*2</f>
         <v>1000</v>
       </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C24" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" s="3" t="n">
         <f aca="false">F14*2</f>
         <v>1000</v>
       </c>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C25" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D25" s="3" t="n">
         <f aca="false">D7*E7*E14</f>
         <v>526.25</v>
       </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D26" s="3" t="n">
         <f aca="false">C7*E7*E14</f>
         <v>526.25</v>
       </c>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="0" t="str">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3" t="str">
         <f aca="false">IF(AND(D21&gt;=0, D22&gt;=1, D21&lt;D23-D25,D22&lt;D24-D26), "Fine", "Too Small")</f>
         <v>Fine</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F19:G27"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>